<commit_message>
data through june 10
</commit_message>
<xml_diff>
--- a/original_spreadsheets/2015/Alachua County Light trap data 2015.xlsx
+++ b/original_spreadsheets/2015/Alachua County Light trap data 2015.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1530" yWindow="-50" windowWidth="15480" windowHeight="7990" tabRatio="833" activeTab="6"/>
+    <workbookView xWindow="1530" yWindow="-50" windowWidth="15480" windowHeight="7990" tabRatio="833" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="blank" sheetId="40" r:id="rId1"/>
@@ -14,12 +14,14 @@
     <sheet name="5-20-15" sheetId="42" r:id="rId5"/>
     <sheet name="5-27-15" sheetId="43" r:id="rId6"/>
     <sheet name="6-2-15" sheetId="44" r:id="rId7"/>
+    <sheet name="6-10-15" sheetId="45" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'5-13-15'!$A$1:$L$41</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">'5-20-15'!$A$1:$L$41</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="5">'5-27-15'!$A$1:$L$41</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'5-6-15'!$A$1:$L$41</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="7">'6-10-15'!$A$1:$L$41</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="6">'6-2-15'!$A$1:$L$41</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">blank!$A$1:$L$39</definedName>
   </definedNames>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="61">
   <si>
     <t>Totals</t>
   </si>
@@ -475,7 +477,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -593,6 +595,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8201,7 +8204,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V144"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
       <selection pane="bottomLeft" activeCell="I33" sqref="I33"/>
@@ -9671,4 +9674,1470 @@
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V144"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.1796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.90625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.54296875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.1796875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="10" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.90625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A1" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="32"/>
+    </row>
+    <row r="2" spans="1:22" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="42"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="30"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A3" s="45">
+        <v>42165</v>
+      </c>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="55" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="29"/>
+    </row>
+    <row r="4" spans="1:22" ht="52" x14ac:dyDescent="0.3">
+      <c r="A4" s="49"/>
+      <c r="B4" s="52" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="52" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="52" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="52" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="52" t="s">
+        <v>56</v>
+      </c>
+      <c r="H4" s="53" t="s">
+        <v>49</v>
+      </c>
+      <c r="I4" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="J4" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="K4" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="L4" s="50"/>
+      <c r="M4" s="50"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A5" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="13">
+        <v>1</v>
+      </c>
+      <c r="C5" s="13">
+        <v>2</v>
+      </c>
+      <c r="D5" s="13">
+        <v>3</v>
+      </c>
+      <c r="E5" s="13">
+        <v>4</v>
+      </c>
+      <c r="F5" s="13">
+        <v>5</v>
+      </c>
+      <c r="G5" s="13">
+        <v>6</v>
+      </c>
+      <c r="H5" s="13">
+        <v>7</v>
+      </c>
+      <c r="I5" s="13">
+        <v>8</v>
+      </c>
+      <c r="J5" s="13">
+        <v>9</v>
+      </c>
+      <c r="K5" s="13">
+        <v>10</v>
+      </c>
+      <c r="L5" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="M5" s="28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A6" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21">
+        <v>1</v>
+      </c>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21">
+        <v>1</v>
+      </c>
+      <c r="L6" s="26">
+        <f>SUM(B6:K6)</f>
+        <v>2</v>
+      </c>
+      <c r="M6" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="26">
+        <f t="shared" ref="L7:L38" si="0">SUM(B7:K7)</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="17">
+        <v>3</v>
+      </c>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="23"/>
+      <c r="S7" s="23"/>
+      <c r="T7" s="23"/>
+      <c r="U7" s="23"/>
+      <c r="V7" s="23"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A8" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19">
+        <v>1</v>
+      </c>
+      <c r="D8" s="19"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18">
+        <v>3</v>
+      </c>
+      <c r="L8" s="26">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M8" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="15.65" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M9" s="17">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A10" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M10" s="17">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A11" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M11" s="17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A12" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M12" s="17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A13" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M13" s="17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A14" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M14" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A15" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M15" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A16" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M16" s="17">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="15">
+        <v>30</v>
+      </c>
+      <c r="C17" s="15">
+        <v>2</v>
+      </c>
+      <c r="D17" s="15"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21">
+        <v>1</v>
+      </c>
+      <c r="G17" s="21">
+        <v>1</v>
+      </c>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21">
+        <v>336</v>
+      </c>
+      <c r="J17" s="21">
+        <v>4</v>
+      </c>
+      <c r="K17" s="21">
+        <v>82</v>
+      </c>
+      <c r="L17" s="26">
+        <f t="shared" si="0"/>
+        <v>456</v>
+      </c>
+      <c r="M17" s="17">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="15">
+        <v>2</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="26">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="M18" s="17">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A19" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="19">
+        <v>8</v>
+      </c>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18">
+        <v>16</v>
+      </c>
+      <c r="K19" s="18"/>
+      <c r="L19" s="26">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="M19" s="17">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A20" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15">
+        <v>7</v>
+      </c>
+      <c r="D20" s="15">
+        <v>3</v>
+      </c>
+      <c r="E20" s="21">
+        <v>1</v>
+      </c>
+      <c r="F20" s="21">
+        <v>2</v>
+      </c>
+      <c r="G20" s="21">
+        <v>3</v>
+      </c>
+      <c r="H20" s="21">
+        <v>10</v>
+      </c>
+      <c r="I20" s="21">
+        <v>80</v>
+      </c>
+      <c r="J20" s="21">
+        <v>352</v>
+      </c>
+      <c r="K20" s="21">
+        <v>48</v>
+      </c>
+      <c r="L20" s="26">
+        <f t="shared" si="0"/>
+        <v>506</v>
+      </c>
+      <c r="M20" s="17">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="19">
+        <v>2</v>
+      </c>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18">
+        <v>1</v>
+      </c>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18">
+        <v>1</v>
+      </c>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18">
+        <v>44</v>
+      </c>
+      <c r="K21" s="18">
+        <v>5</v>
+      </c>
+      <c r="L21" s="26">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="M21" s="17">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A22" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M22" s="17">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A23" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M23" s="17">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A24" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M24" s="17">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A25" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M25" s="17">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="15">
+        <v>6</v>
+      </c>
+      <c r="C26" s="15">
+        <v>2</v>
+      </c>
+      <c r="D26" s="15"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21">
+        <v>3</v>
+      </c>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21">
+        <v>25</v>
+      </c>
+      <c r="I26" s="21">
+        <v>592</v>
+      </c>
+      <c r="J26" s="21">
+        <v>96</v>
+      </c>
+      <c r="K26" s="21">
+        <v>28</v>
+      </c>
+      <c r="L26" s="26">
+        <f t="shared" si="0"/>
+        <v>752</v>
+      </c>
+      <c r="M26" s="17">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A27" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M27" s="17">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A28" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15">
+        <v>1</v>
+      </c>
+      <c r="D28" s="15"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21">
+        <v>1</v>
+      </c>
+      <c r="H28" s="21">
+        <v>5</v>
+      </c>
+      <c r="I28" s="21">
+        <v>64</v>
+      </c>
+      <c r="J28" s="21">
+        <v>104</v>
+      </c>
+      <c r="K28" s="21">
+        <v>7</v>
+      </c>
+      <c r="L28" s="26">
+        <f t="shared" si="0"/>
+        <v>182</v>
+      </c>
+      <c r="M28" s="17">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M29" s="17">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A30" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="15">
+        <v>2</v>
+      </c>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15">
+        <v>2</v>
+      </c>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="21"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="26">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M30" s="17">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A31" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="21"/>
+      <c r="L31" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M31" s="17">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A32" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="21"/>
+      <c r="K32" s="21"/>
+      <c r="L32" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M32" s="17">
+        <v>54</v>
+      </c>
+      <c r="S32" s="35"/>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A33" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M33" s="17">
+        <v>88</v>
+      </c>
+      <c r="S33" s="35"/>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A34" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="18"/>
+      <c r="K34" s="18"/>
+      <c r="L34" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M34" s="17">
+        <v>70</v>
+      </c>
+      <c r="S34" s="35"/>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A35" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35" s="19"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="18"/>
+      <c r="K35" s="18"/>
+      <c r="L35" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M35" s="17">
+        <v>71</v>
+      </c>
+      <c r="S35" s="35"/>
+    </row>
+    <row r="36" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" s="19"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="18"/>
+      <c r="L36" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M36" s="17">
+        <v>80</v>
+      </c>
+      <c r="S36" s="35"/>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A37" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="37"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="18"/>
+      <c r="J37" s="18"/>
+      <c r="K37" s="18"/>
+      <c r="L37" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M37" s="17">
+        <v>82</v>
+      </c>
+      <c r="S37" s="35"/>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A38" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" s="37"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
+      <c r="I38" s="18"/>
+      <c r="J38" s="18"/>
+      <c r="K38" s="18"/>
+      <c r="L38" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M38" s="17">
+        <v>100</v>
+      </c>
+      <c r="S38" s="35"/>
+    </row>
+    <row r="39" spans="1:19" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" s="16">
+        <f>SUM(B6:B38)</f>
+        <v>50</v>
+      </c>
+      <c r="C39" s="16">
+        <f t="shared" ref="C39:L39" si="1">SUM(C6:C38)</f>
+        <v>13</v>
+      </c>
+      <c r="D39" s="16">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="E39" s="16">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F39" s="16">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="G39" s="16">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="H39" s="16">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="I39" s="16">
+        <f t="shared" si="1"/>
+        <v>1072</v>
+      </c>
+      <c r="J39" s="16">
+        <f t="shared" si="1"/>
+        <v>616</v>
+      </c>
+      <c r="K39" s="16">
+        <f t="shared" si="1"/>
+        <v>174</v>
+      </c>
+      <c r="L39" s="16">
+        <f t="shared" si="1"/>
+        <v>1985</v>
+      </c>
+      <c r="M39" s="14"/>
+      <c r="S39" s="35"/>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A40" s="12"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="4"/>
+      <c r="P40" s="35"/>
+    </row>
+    <row r="41" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="9"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="4"/>
+      <c r="P41" s="35"/>
+    </row>
+    <row r="42" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="5"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="P42" s="35"/>
+    </row>
+    <row r="43" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="5"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="P43" s="35"/>
+    </row>
+    <row r="44" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="5"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
+      <c r="P44" s="35"/>
+    </row>
+    <row r="45" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="5"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="P45" s="35"/>
+    </row>
+    <row r="46" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="5"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+      <c r="P46" s="35"/>
+    </row>
+    <row r="47" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="5"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="P47" s="35"/>
+    </row>
+    <row r="48" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="5"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="P48" s="35"/>
+    </row>
+    <row r="49" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="5"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="P49" s="35"/>
+    </row>
+    <row r="50" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="5"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="P50" s="35"/>
+    </row>
+    <row r="51" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="5"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
+      <c r="P51" s="35"/>
+    </row>
+    <row r="52" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="5"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+      <c r="P52" s="35"/>
+    </row>
+    <row r="53" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="5"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+      <c r="P53" s="35"/>
+    </row>
+    <row r="54" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="5"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+      <c r="P54" s="35"/>
+    </row>
+    <row r="55" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="5"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
+      <c r="H55" s="4"/>
+      <c r="P55" s="35"/>
+    </row>
+    <row r="56" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="5"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="4"/>
+      <c r="D56" s="4"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+      <c r="P56" s="35"/>
+    </row>
+    <row r="57" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="5"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="P57" s="35"/>
+    </row>
+    <row r="58" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="5"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
+      <c r="G58" s="4"/>
+      <c r="H58" s="4"/>
+      <c r="P58" s="35"/>
+    </row>
+    <row r="59" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="5"/>
+      <c r="B59" s="4"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="4"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="4"/>
+      <c r="G59" s="4"/>
+      <c r="H59" s="4"/>
+      <c r="P59" s="35"/>
+    </row>
+    <row r="60" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="5"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="4"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+      <c r="P60" s="35"/>
+    </row>
+    <row r="61" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="5"/>
+      <c r="B61" s="4"/>
+      <c r="C61" s="4"/>
+      <c r="D61" s="4"/>
+      <c r="E61" s="4"/>
+      <c r="F61" s="4"/>
+      <c r="G61" s="4"/>
+      <c r="H61" s="4"/>
+      <c r="P61" s="35"/>
+    </row>
+    <row r="62" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="5"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="4"/>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4"/>
+      <c r="G62" s="4"/>
+      <c r="H62" s="4"/>
+      <c r="P62" s="35"/>
+    </row>
+    <row r="63" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="5"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="4"/>
+      <c r="E63" s="4"/>
+      <c r="F63" s="4"/>
+      <c r="G63" s="4"/>
+      <c r="H63" s="4"/>
+    </row>
+    <row r="64" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="5"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="4"/>
+      <c r="D64" s="4"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4"/>
+      <c r="G64" s="4"/>
+      <c r="H64" s="4"/>
+    </row>
+    <row r="65" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="5"/>
+      <c r="B65" s="4"/>
+      <c r="C65" s="4"/>
+      <c r="D65" s="4"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="4"/>
+      <c r="G65" s="4"/>
+      <c r="H65" s="4"/>
+    </row>
+    <row r="66" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="5"/>
+      <c r="B66" s="4"/>
+      <c r="C66" s="4"/>
+      <c r="D66" s="4"/>
+      <c r="E66" s="4"/>
+      <c r="F66" s="4"/>
+      <c r="G66" s="4"/>
+      <c r="H66" s="4"/>
+    </row>
+    <row r="67" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="5"/>
+      <c r="B67" s="4"/>
+      <c r="C67" s="4"/>
+      <c r="D67" s="4"/>
+      <c r="E67" s="4"/>
+      <c r="F67" s="4"/>
+      <c r="G67" s="4"/>
+      <c r="H67" s="4"/>
+    </row>
+    <row r="68" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="5"/>
+      <c r="B68" s="4"/>
+      <c r="C68" s="4"/>
+      <c r="D68" s="4"/>
+      <c r="E68" s="4"/>
+      <c r="F68" s="4"/>
+      <c r="G68" s="4"/>
+      <c r="H68" s="4"/>
+    </row>
+    <row r="69" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="5"/>
+      <c r="B69" s="6"/>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="6"/>
+    </row>
+    <row r="70" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="3"/>
+      <c r="B70" s="4"/>
+      <c r="C70" s="4"/>
+      <c r="D70" s="4"/>
+      <c r="E70" s="4"/>
+      <c r="F70" s="4"/>
+      <c r="G70" s="4"/>
+    </row>
+    <row r="71" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="3"/>
+      <c r="B71" s="4"/>
+      <c r="C71" s="4"/>
+      <c r="D71" s="4"/>
+      <c r="E71" s="4"/>
+      <c r="F71" s="4"/>
+      <c r="G71" s="4"/>
+    </row>
+    <row r="72" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="5"/>
+      <c r="B72" s="4"/>
+      <c r="C72" s="4"/>
+      <c r="D72" s="4"/>
+      <c r="E72" s="4"/>
+      <c r="F72" s="4"/>
+      <c r="G72" s="4"/>
+    </row>
+    <row r="73" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="3"/>
+    </row>
+    <row r="74" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="75" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="76" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="77" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="78" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="79" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="80" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="81" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="82" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="83" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="84" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="85" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="86" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="87" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="88" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="89" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="90" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="91" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="92" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="93" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="94" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="95" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="96" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="97" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="98" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="99" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="100" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="101" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="102" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="103" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="104" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="105" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="106" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="107" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="108" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="109" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="110" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="111" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="112" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="113" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="114" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="115" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="116" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="117" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="118" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="119" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="120" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="121" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="122" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="123" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="124" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="125" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="126" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="127" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="128" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="129" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="130" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="131" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="132" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="133" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="134" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="135" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="136" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="137" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="138" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="139" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="140" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="141" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="142" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="143" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B143" s="1"/>
+      <c r="C143" s="1"/>
+      <c r="D143" s="1"/>
+      <c r="E143" s="1"/>
+      <c r="F143" s="1"/>
+      <c r="G143" s="1"/>
+      <c r="H143" s="1"/>
+    </row>
+    <row r="144" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A144" s="1"/>
+      <c r="B144" s="1"/>
+      <c r="C144" s="1"/>
+      <c r="D144" s="1"/>
+      <c r="E144" s="1"/>
+      <c r="F144" s="1"/>
+      <c r="G144" s="1"/>
+      <c r="H144" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="300" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
 </file>
</xml_diff>